<commit_message>
majors to job csvs
</commit_message>
<xml_diff>
--- a/data/raw/Majors_Ocupations_Mapping.xlsx
+++ b/data/raw/Majors_Ocupations_Mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DataBootcamp\Group Project\Final Project\FortunED\data\raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swati\Documents\GitHub\FortunED\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B28A781B-718B-48DE-A4BA-28CBBCCBB9CA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C769D6FD-1081-4DDF-A00C-A4013F05DB0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A059D824-750F-4FF3-A414-8E73938B05E8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A059D824-750F-4FF3-A414-8E73938B05E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -78,46 +78,46 @@
     <t>Social Science</t>
   </si>
   <si>
-    <t>1-0000  Management Occupations</t>
-  </si>
-  <si>
-    <t>13-0000  Business and Financial Operations Occupations</t>
-  </si>
-  <si>
-    <t>15-0000  Computer and Mathematical Occupations</t>
-  </si>
-  <si>
-    <t>17-0000  Architecture and Engineering Occupations</t>
-  </si>
-  <si>
-    <t>19-0000  Life, Physical, and Social Science Occupations</t>
-  </si>
-  <si>
-    <t>21-0000  Community and Social Service Occupations</t>
-  </si>
-  <si>
-    <t>23-0000  Legal Occupations</t>
-  </si>
-  <si>
-    <t>25-0000  Educational Instruction and Library Occupations</t>
-  </si>
-  <si>
-    <t>27-0000  Arts, Design, Entertainment, Sports, and Media Occupations</t>
-  </si>
-  <si>
-    <t>29-0000  Healthcare Practitioners and Technical Occupations</t>
-  </si>
-  <si>
-    <t>31-0000  Healthcare Support Occupations</t>
-  </si>
-  <si>
-    <t>45-0000  Farming, Fishing, and Forestry Occupations</t>
-  </si>
-  <si>
     <t>Major Category</t>
   </si>
   <si>
     <t>Ocupation industry</t>
+  </si>
+  <si>
+    <t>Farming, Fishing, and Forestry Occupations</t>
+  </si>
+  <si>
+    <t>Arts, Design, Entertainment, Sports, and Media Occupations</t>
+  </si>
+  <si>
+    <t>Business and Financial Operations Occupations</t>
+  </si>
+  <si>
+    <t>Management Occupations</t>
+  </si>
+  <si>
+    <t>Computer and Mathematical Occupations</t>
+  </si>
+  <si>
+    <t>Educational Instruction and Library Occupations</t>
+  </si>
+  <si>
+    <t>Architecture and Engineering Occupations</t>
+  </si>
+  <si>
+    <t>Healthcare Practitioners and Technical Occupations</t>
+  </si>
+  <si>
+    <t>Healthcare Support Occupations</t>
+  </si>
+  <si>
+    <t>Legal Occupations</t>
+  </si>
+  <si>
+    <t>Community and Social Service Occupations</t>
+  </si>
+  <si>
+    <t>Life, Physical, and Social Science Occupations</t>
   </si>
 </sst>
 </file>
@@ -481,89 +481,89 @@
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:B34"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="64.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="64.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -571,15 +571,15 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -587,7 +587,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -595,47 +595,47 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
     </row>
   </sheetData>

</xml_diff>